<commit_message>
First cut at getting boats moving around on the screen.  Yesssssss.....
</commit_message>
<xml_diff>
--- a/icons/icons.xlsx
+++ b/icons/icons.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>U</t>
   </si>
@@ -31,6 +31,27 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>num vals for 180 degs</t>
+  </si>
+  <si>
+    <t>earth circumference in meters</t>
+  </si>
+  <si>
+    <t>meters per degree</t>
+  </si>
+  <si>
+    <t>meters per tick</t>
+  </si>
+  <si>
+    <t>ticks per degree</t>
+  </si>
+  <si>
+    <t>num degrees</t>
+  </si>
+  <si>
+    <t>mm per tick</t>
   </si>
 </sst>
 </file>
@@ -476,13 +497,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G1:K1"/>
+  <dimension ref="G1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="7:11" ht="61" customHeight="1">
       <c r="G1" s="1" t="s">
@@ -498,6 +523,67 @@
         <v>3</v>
       </c>
       <c r="K1" s="4"/>
+    </row>
+    <row r="5" spans="7:11">
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="7:11">
+      <c r="G6">
+        <f>POWER(2, 31)</f>
+        <v>2147483648</v>
+      </c>
+      <c r="H6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="7:11">
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <f>G6/H6</f>
+        <v>11930464.711111112</v>
+      </c>
+    </row>
+    <row r="10" spans="7:11">
+      <c r="G10">
+        <v>40075000</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="7:11">
+      <c r="G11">
+        <f>G10/360</f>
+        <v>111319.44444444444</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="7:11">
+      <c r="G13">
+        <f>G11/H8</f>
+        <v>9.3306880444288236E-3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="7:11">
+      <c r="G14">
+        <f>G13*1000</f>
+        <v>9.3306880444288236</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>